<commit_message>
Got some work done.
</commit_message>
<xml_diff>
--- a/Data Attributes.xlsx
+++ b/Data Attributes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marin Family\Desktop\SMU Coursework\Data Mining\Costa Rican Poverty Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82B06E2-8022-49E0-B570-A393BA4A1709}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F58BDF-A5E4-4E0F-8409-4601C6F558ED}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7995" xr2:uid="{1A8029D2-DA50-4944-9503-F4FE15AE9DC8}"/>
   </bookViews>
@@ -1260,7 +1260,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF1C28E-C172-45FF-91AE-6E4AC7D0B71B}">
   <dimension ref="A1:C142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Checking in Sunday's Work.
</commit_message>
<xml_diff>
--- a/Data Attributes.xlsx
+++ b/Data Attributes.xlsx
@@ -1,24 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marin Family\Desktop\SMU Coursework\Data Mining\Costa Rican Poverty Prediction\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F58BDF-A5E4-4E0F-8409-4601C6F558ED}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7995" xr2:uid="{1A8029D2-DA50-4944-9503-F4FE15AE9DC8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$142</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$142</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="293">
   <si>
     <t>v2a1</t>
   </si>
@@ -898,12 +892,21 @@
   </si>
   <si>
     <t>numeric</t>
+  </si>
+  <si>
+    <t>Household Level</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Member Level</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1250,28 +1253,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF1C28E-C172-45FF-91AE-6E4AC7D0B71B}">
-  <dimension ref="A1:C142"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="C139" sqref="C139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="146.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="52.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>273</v>
       </c>
@@ -1279,10 +1283,13 @@
         <v>274</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1290,10 +1297,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D2" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1301,10 +1311,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1312,10 +1325,13 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
+        <v>290</v>
+      </c>
+      <c r="D4" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1323,10 +1339,13 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1334,10 +1353,13 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D6" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1345,10 +1367,13 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1356,10 +1381,13 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D8" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1367,10 +1395,13 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
+        <v>290</v>
+      </c>
+      <c r="D9" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1378,10 +1409,13 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
+        <v>290</v>
+      </c>
+      <c r="D10" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1389,10 +1423,13 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
+        <v>290</v>
+      </c>
+      <c r="D11" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1400,10 +1437,13 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
+        <v>290</v>
+      </c>
+      <c r="D12" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1411,10 +1451,13 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
+        <v>290</v>
+      </c>
+      <c r="D13" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1422,10 +1465,13 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
+        <v>290</v>
+      </c>
+      <c r="D14" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1433,10 +1479,13 @@
         <v>27</v>
       </c>
       <c r="C15" t="s">
+        <v>290</v>
+      </c>
+      <c r="D15" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1444,10 +1493,13 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
+        <v>290</v>
+      </c>
+      <c r="D16" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1455,10 +1507,13 @@
         <v>31</v>
       </c>
       <c r="C17" t="s">
+        <v>290</v>
+      </c>
+      <c r="D17" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1466,10 +1521,13 @@
         <v>33</v>
       </c>
       <c r="C18" t="s">
+        <v>290</v>
+      </c>
+      <c r="D18" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1477,10 +1535,13 @@
         <v>35</v>
       </c>
       <c r="C19" t="s">
+        <v>290</v>
+      </c>
+      <c r="D19" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1488,10 +1549,13 @@
         <v>37</v>
       </c>
       <c r="C20" t="s">
+        <v>290</v>
+      </c>
+      <c r="D20" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1499,10 +1563,13 @@
         <v>39</v>
       </c>
       <c r="C21" t="s">
+        <v>292</v>
+      </c>
+      <c r="D21" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -1510,10 +1577,13 @@
         <v>41</v>
       </c>
       <c r="C22" t="s">
+        <v>292</v>
+      </c>
+      <c r="D22" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1521,10 +1591,13 @@
         <v>43</v>
       </c>
       <c r="C23" t="s">
+        <v>292</v>
+      </c>
+      <c r="D23" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1532,10 +1605,13 @@
         <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D24" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1543,10 +1619,13 @@
         <v>276</v>
       </c>
       <c r="C25" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D25" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -1554,10 +1633,13 @@
         <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D26" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -1565,10 +1647,13 @@
         <v>50</v>
       </c>
       <c r="C27" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D27" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>51</v>
       </c>
@@ -1576,10 +1661,13 @@
         <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D28" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -1587,10 +1675,13 @@
         <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D29" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1598,10 +1689,13 @@
         <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D30" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -1609,10 +1703,13 @@
         <v>58</v>
       </c>
       <c r="C31" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D31" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -1620,10 +1717,13 @@
         <v>279</v>
       </c>
       <c r="C32" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D32" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>60</v>
       </c>
@@ -1631,10 +1731,13 @@
         <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D33" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>62</v>
       </c>
@@ -1642,10 +1745,13 @@
         <v>63</v>
       </c>
       <c r="C34" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D34" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -1653,10 +1759,13 @@
         <v>65</v>
       </c>
       <c r="C35" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D35" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>66</v>
       </c>
@@ -1664,10 +1773,13 @@
         <v>67</v>
       </c>
       <c r="C36" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D36" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>68</v>
       </c>
@@ -1675,10 +1787,13 @@
         <v>69</v>
       </c>
       <c r="C37" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D37" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>70</v>
       </c>
@@ -1686,10 +1801,13 @@
         <v>71</v>
       </c>
       <c r="C38" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D38" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>72</v>
       </c>
@@ -1697,10 +1815,13 @@
         <v>278</v>
       </c>
       <c r="C39" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D39" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>73</v>
       </c>
@@ -1708,10 +1829,13 @@
         <v>74</v>
       </c>
       <c r="C40" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>75</v>
       </c>
@@ -1719,10 +1843,13 @@
         <v>76</v>
       </c>
       <c r="C41" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D41" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>77</v>
       </c>
@@ -1730,10 +1857,13 @@
         <v>78</v>
       </c>
       <c r="C42" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D42" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>79</v>
       </c>
@@ -1741,10 +1871,13 @@
         <v>80</v>
       </c>
       <c r="C43" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D43" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>81</v>
       </c>
@@ -1752,10 +1885,13 @@
         <v>82</v>
       </c>
       <c r="C44" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D44" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>83</v>
       </c>
@@ -1763,10 +1899,13 @@
         <v>84</v>
       </c>
       <c r="C45" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D45" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>85</v>
       </c>
@@ -1774,10 +1913,13 @@
         <v>277</v>
       </c>
       <c r="C46" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D46" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>86</v>
       </c>
@@ -1785,10 +1927,13 @@
         <v>87</v>
       </c>
       <c r="C47" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D47" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>88</v>
       </c>
@@ -1796,10 +1941,13 @@
         <v>89</v>
       </c>
       <c r="C48" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D48" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>90</v>
       </c>
@@ -1807,10 +1955,13 @@
         <v>91</v>
       </c>
       <c r="C49" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D49" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>92</v>
       </c>
@@ -1818,10 +1969,13 @@
         <v>93</v>
       </c>
       <c r="C50" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D50" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>94</v>
       </c>
@@ -1829,10 +1983,13 @@
         <v>95</v>
       </c>
       <c r="C51" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D51" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>96</v>
       </c>
@@ -1840,10 +1997,13 @@
         <v>97</v>
       </c>
       <c r="C52" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D52" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>98</v>
       </c>
@@ -1851,10 +2011,13 @@
         <v>99</v>
       </c>
       <c r="C53" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D53" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>100</v>
       </c>
@@ -1862,10 +2025,13 @@
         <v>101</v>
       </c>
       <c r="C54" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D54" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>102</v>
       </c>
@@ -1873,10 +2039,13 @@
         <v>103</v>
       </c>
       <c r="C55" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D55" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>104</v>
       </c>
@@ -1884,10 +2053,13 @@
         <v>105</v>
       </c>
       <c r="C56" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D56" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>106</v>
       </c>
@@ -1895,10 +2067,13 @@
         <v>107</v>
       </c>
       <c r="C57" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D57" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>108</v>
       </c>
@@ -1906,10 +2081,13 @@
         <v>109</v>
       </c>
       <c r="C58" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D58" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -1917,10 +2095,13 @@
         <v>111</v>
       </c>
       <c r="C59" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D59" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>112</v>
       </c>
@@ -1928,10 +2109,13 @@
         <v>113</v>
       </c>
       <c r="C60" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D60" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>114</v>
       </c>
@@ -1939,10 +2123,13 @@
         <v>115</v>
       </c>
       <c r="C61" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D61" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>116</v>
       </c>
@@ -1950,10 +2137,13 @@
         <v>117</v>
       </c>
       <c r="C62" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D62" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>118</v>
       </c>
@@ -1961,10 +2151,13 @@
         <v>119</v>
       </c>
       <c r="C63" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D63" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>120</v>
       </c>
@@ -1972,10 +2165,13 @@
         <v>121</v>
       </c>
       <c r="C64" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D64" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>122</v>
       </c>
@@ -1983,10 +2179,13 @@
         <v>123</v>
       </c>
       <c r="C65" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D65" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>124</v>
       </c>
@@ -1994,10 +2193,13 @@
         <v>125</v>
       </c>
       <c r="C66" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D66" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>126</v>
       </c>
@@ -2005,10 +2207,13 @@
         <v>127</v>
       </c>
       <c r="C67" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D67" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>128</v>
       </c>
@@ -2016,10 +2221,13 @@
         <v>129</v>
       </c>
       <c r="C68" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D68" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>130</v>
       </c>
@@ -2027,10 +2235,13 @@
         <v>131</v>
       </c>
       <c r="C69" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D69" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>132</v>
       </c>
@@ -2038,10 +2249,13 @@
         <v>133</v>
       </c>
       <c r="C70" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D70" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>134</v>
       </c>
@@ -2049,10 +2263,13 @@
         <v>135</v>
       </c>
       <c r="C71" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D71" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>136</v>
       </c>
@@ -2060,10 +2277,13 @@
         <v>137</v>
       </c>
       <c r="C72" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D72" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>138</v>
       </c>
@@ -2071,10 +2291,13 @@
         <v>139</v>
       </c>
       <c r="C73" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D73" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>140</v>
       </c>
@@ -2082,10 +2305,13 @@
         <v>141</v>
       </c>
       <c r="C74" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D74" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>142</v>
       </c>
@@ -2093,10 +2319,13 @@
         <v>143</v>
       </c>
       <c r="C75" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D75" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>144</v>
       </c>
@@ -2104,10 +2333,13 @@
         <v>145</v>
       </c>
       <c r="C76" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D76" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>146</v>
       </c>
@@ -2115,10 +2347,13 @@
         <v>147</v>
       </c>
       <c r="C77" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D77" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>148</v>
       </c>
@@ -2126,10 +2361,13 @@
         <v>149</v>
       </c>
       <c r="C78" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D78" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>150</v>
       </c>
@@ -2137,10 +2375,13 @@
         <v>151</v>
       </c>
       <c r="C79" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D79" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>152</v>
       </c>
@@ -2148,10 +2389,13 @@
         <v>153</v>
       </c>
       <c r="C80" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D80" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>154</v>
       </c>
@@ -2159,10 +2403,13 @@
         <v>155</v>
       </c>
       <c r="C81" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D81" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>156</v>
       </c>
@@ -2170,10 +2417,13 @@
         <v>157</v>
       </c>
       <c r="C82" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D82" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>158</v>
       </c>
@@ -2181,10 +2431,13 @@
         <v>159</v>
       </c>
       <c r="C83" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D83" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>160</v>
       </c>
@@ -2192,10 +2445,13 @@
         <v>161</v>
       </c>
       <c r="C84" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D84" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>162</v>
       </c>
@@ -2203,10 +2459,13 @@
         <v>163</v>
       </c>
       <c r="C85" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D85" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>164</v>
       </c>
@@ -2214,10 +2473,13 @@
         <v>165</v>
       </c>
       <c r="C86" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D86" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>166</v>
       </c>
@@ -2225,10 +2487,13 @@
         <v>167</v>
       </c>
       <c r="C87" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D87" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>168</v>
       </c>
@@ -2236,10 +2501,13 @@
         <v>169</v>
       </c>
       <c r="C88" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D88" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>170</v>
       </c>
@@ -2247,10 +2515,13 @@
         <v>171</v>
       </c>
       <c r="C89" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D89" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>172</v>
       </c>
@@ -2258,10 +2529,13 @@
         <v>173</v>
       </c>
       <c r="C90" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D90" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>174</v>
       </c>
@@ -2269,10 +2543,13 @@
         <v>175</v>
       </c>
       <c r="C91" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D91" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>176</v>
       </c>
@@ -2280,10 +2557,13 @@
         <v>177</v>
       </c>
       <c r="C92" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D92" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>178</v>
       </c>
@@ -2291,10 +2571,13 @@
         <v>179</v>
       </c>
       <c r="C93" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D93" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>180</v>
       </c>
@@ -2302,10 +2585,13 @@
         <v>181</v>
       </c>
       <c r="C94" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D94" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>182</v>
       </c>
@@ -2313,10 +2599,13 @@
         <v>183</v>
       </c>
       <c r="C95" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D95" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>184</v>
       </c>
@@ -2324,10 +2613,13 @@
         <v>185</v>
       </c>
       <c r="C96" t="s">
+        <v>290</v>
+      </c>
+      <c r="D96" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>186</v>
       </c>
@@ -2335,10 +2627,13 @@
         <v>187</v>
       </c>
       <c r="C97" t="s">
+        <v>290</v>
+      </c>
+      <c r="D97" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>188</v>
       </c>
@@ -2346,10 +2641,13 @@
         <v>189</v>
       </c>
       <c r="C98" t="s">
+        <v>290</v>
+      </c>
+      <c r="D98" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>190</v>
       </c>
@@ -2357,10 +2655,13 @@
         <v>191</v>
       </c>
       <c r="C99" t="s">
+        <v>290</v>
+      </c>
+      <c r="D99" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>192</v>
       </c>
@@ -2368,10 +2669,13 @@
         <v>193</v>
       </c>
       <c r="C100" t="s">
+        <v>290</v>
+      </c>
+      <c r="D100" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>194</v>
       </c>
@@ -2379,10 +2683,13 @@
         <v>283</v>
       </c>
       <c r="C101" t="s">
+        <v>290</v>
+      </c>
+      <c r="D101" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>195</v>
       </c>
@@ -2390,10 +2697,13 @@
         <v>284</v>
       </c>
       <c r="C102" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D102" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>196</v>
       </c>
@@ -2401,10 +2711,13 @@
         <v>285</v>
       </c>
       <c r="C103" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D103" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>197</v>
       </c>
@@ -2412,10 +2725,13 @@
         <v>198</v>
       </c>
       <c r="C104" t="s">
+        <v>290</v>
+      </c>
+      <c r="D104" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>199</v>
       </c>
@@ -2423,10 +2739,13 @@
         <v>200</v>
       </c>
       <c r="C105" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D105" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>201</v>
       </c>
@@ -2434,10 +2753,13 @@
         <v>202</v>
       </c>
       <c r="C106" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D106" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>203</v>
       </c>
@@ -2445,10 +2767,13 @@
         <v>204</v>
       </c>
       <c r="C107" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D107" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>205</v>
       </c>
@@ -2456,10 +2781,13 @@
         <v>206</v>
       </c>
       <c r="C108" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D108" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>207</v>
       </c>
@@ -2467,10 +2795,13 @@
         <v>208</v>
       </c>
       <c r="C109" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D109" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>209</v>
       </c>
@@ -2478,10 +2809,13 @@
         <v>210</v>
       </c>
       <c r="C110" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D110" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>211</v>
       </c>
@@ -2489,10 +2823,13 @@
         <v>212</v>
       </c>
       <c r="C111" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D111" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>213</v>
       </c>
@@ -2500,10 +2837,13 @@
         <v>214</v>
       </c>
       <c r="C112" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D112" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>215</v>
       </c>
@@ -2511,10 +2851,13 @@
         <v>216</v>
       </c>
       <c r="C113" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D113" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>217</v>
       </c>
@@ -2522,10 +2865,13 @@
         <v>218</v>
       </c>
       <c r="C114" t="s">
+        <v>290</v>
+      </c>
+      <c r="D114" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>219</v>
       </c>
@@ -2533,10 +2879,13 @@
         <v>220</v>
       </c>
       <c r="C115" t="s">
+        <v>290</v>
+      </c>
+      <c r="D115" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>221</v>
       </c>
@@ -2544,10 +2893,13 @@
         <v>222</v>
       </c>
       <c r="C116" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D116" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>223</v>
       </c>
@@ -2555,10 +2907,13 @@
         <v>280</v>
       </c>
       <c r="C117" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D117" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>224</v>
       </c>
@@ -2566,10 +2921,13 @@
         <v>225</v>
       </c>
       <c r="C118" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D118" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>226</v>
       </c>
@@ -2577,10 +2935,13 @@
         <v>227</v>
       </c>
       <c r="C119" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D119" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>228</v>
       </c>
@@ -2588,10 +2949,13 @@
         <v>281</v>
       </c>
       <c r="C120" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D120" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>229</v>
       </c>
@@ -2599,10 +2963,13 @@
         <v>230</v>
       </c>
       <c r="C121" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D121" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>231</v>
       </c>
@@ -2610,10 +2977,13 @@
         <v>232</v>
       </c>
       <c r="C122" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D122" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>233</v>
       </c>
@@ -2621,10 +2991,13 @@
         <v>234</v>
       </c>
       <c r="C123" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D123" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>235</v>
       </c>
@@ -2632,10 +3005,13 @@
         <v>236</v>
       </c>
       <c r="C124" t="s">
+        <v>290</v>
+      </c>
+      <c r="D124" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>237</v>
       </c>
@@ -2643,10 +3019,13 @@
         <v>238</v>
       </c>
       <c r="C125" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D125" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>239</v>
       </c>
@@ -2654,10 +3033,13 @@
         <v>240</v>
       </c>
       <c r="C126" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D126" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>241</v>
       </c>
@@ -2665,10 +3047,13 @@
         <v>242</v>
       </c>
       <c r="C127" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D127" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>243</v>
       </c>
@@ -2676,10 +3061,13 @@
         <v>244</v>
       </c>
       <c r="C128" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D128" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>245</v>
       </c>
@@ -2687,10 +3075,13 @@
         <v>246</v>
       </c>
       <c r="C129" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D129" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>247</v>
       </c>
@@ -2698,10 +3089,13 @@
         <v>248</v>
       </c>
       <c r="C130" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D130" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>249</v>
       </c>
@@ -2709,10 +3103,13 @@
         <v>250</v>
       </c>
       <c r="C131" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D131" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>251</v>
       </c>
@@ -2720,10 +3117,13 @@
         <v>252</v>
       </c>
       <c r="C132" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D132" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>253</v>
       </c>
@@ -2731,10 +3131,13 @@
         <v>254</v>
       </c>
       <c r="C133" t="s">
+        <v>290</v>
+      </c>
+      <c r="D133" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>255</v>
       </c>
@@ -2742,10 +3145,13 @@
         <v>256</v>
       </c>
       <c r="C134" t="s">
+        <v>290</v>
+      </c>
+      <c r="D134" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>257</v>
       </c>
@@ -2753,10 +3159,13 @@
         <v>258</v>
       </c>
       <c r="C135" t="s">
+        <v>290</v>
+      </c>
+      <c r="D135" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>259</v>
       </c>
@@ -2764,10 +3173,13 @@
         <v>260</v>
       </c>
       <c r="C136" t="s">
+        <v>290</v>
+      </c>
+      <c r="D136" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>261</v>
       </c>
@@ -2775,10 +3187,13 @@
         <v>262</v>
       </c>
       <c r="C137" t="s">
+        <v>290</v>
+      </c>
+      <c r="D137" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>263</v>
       </c>
@@ -2786,10 +3201,13 @@
         <v>264</v>
       </c>
       <c r="C138" t="s">
+        <v>290</v>
+      </c>
+      <c r="D138" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>265</v>
       </c>
@@ -2797,10 +3215,13 @@
         <v>266</v>
       </c>
       <c r="C139" t="s">
+        <v>290</v>
+      </c>
+      <c r="D139" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>267</v>
       </c>
@@ -2808,10 +3229,13 @@
         <v>268</v>
       </c>
       <c r="C140" t="s">
+        <v>290</v>
+      </c>
+      <c r="D140" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>269</v>
       </c>
@@ -2819,10 +3243,13 @@
         <v>270</v>
       </c>
       <c r="C141" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D141" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>271</v>
       </c>
@@ -2830,11 +3257,14 @@
         <v>272</v>
       </c>
       <c r="C142" t="s">
+        <v>290</v>
+      </c>
+      <c r="D142" t="s">
         <v>289</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C142" xr:uid="{E22A7E0F-157C-4D35-910B-CDA3FB73E9D5}"/>
+  <autoFilter ref="A1:D142"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>